<commit_message>
Actualización: se añaden respaldos de datos, nuevas configuraciones, y ajustes en scripts
</commit_message>
<xml_diff>
--- a/docs/normalizacion_tablas.xlsx
+++ b/docs/normalizacion_tablas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Documents\GitHub - Projects\Doc-UP-AlejandroJaimes\BDI-GB-ZOO\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin Ramirez\Documents\Git\GitHub\Kevin Ramirez\BDI-GB-ZOO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9344971C-90BD-4479-A62A-4ED9681A31F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3070EA7A-9496-4FA2-AA0F-F9C83082A69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11640" yWindow="0" windowWidth="11496" windowHeight="14496" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalizacion" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -415,6 +415,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -445,8 +446,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -834,54 +833,54 @@
   <dimension ref="C2:I8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:9" ht="18.600000000000001">
-      <c r="C2" s="14" t="s">
+    <row r="2" spans="3:9" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="3:9">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="3:9">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="3:9">
-      <c r="C5" s="17" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="12" t="str">
         <f>HYPERLINK("[FormasNormales.xlsx]1FN!B1","1FN")</f>
         <v>1FN</v>
@@ -899,10 +898,10 @@
         <v>4FN</v>
       </c>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="3:9">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E8" s="13"/>
     </row>
   </sheetData>
@@ -921,81 +920,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA81C315-C728-4E3C-8771-B82AD9D270EA}">
   <dimension ref="B1:U11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="59" workbookViewId="0">
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.09765625" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="4" max="4" width="10.09765625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" customWidth="1"/>
-    <col min="10" max="10" width="19.69921875" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" customWidth="1"/>
-    <col min="16" max="16" width="12.09765625" customWidth="1"/>
-    <col min="19" max="19" width="13.796875" customWidth="1"/>
-    <col min="20" max="20" width="15.69921875" customWidth="1"/>
-    <col min="21" max="21" width="15.09765625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.77734375" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-    </row>
-    <row r="2" spans="2:21">
-      <c r="B2" s="20" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="2:21">
-      <c r="S3" s="24"/>
-    </row>
-    <row r="4" spans="2:21">
-      <c r="B4" s="19" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="F4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="J4" s="19" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="J4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="N4" s="19" t="s">
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="N4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="S4" s="19" t="s">
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="S4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="5" spans="2:21">
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1042,7 +1041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:21">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1089,7 +1088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:21">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:21">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:21">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:21">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:21">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1287,79 +1286,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D3B809-3E7B-4F7C-A7F4-3DC96BDFA24D}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="52" workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.09765625" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="4" max="4" width="10.09765625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" customWidth="1"/>
-    <col min="10" max="10" width="19.69921875" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" customWidth="1"/>
-    <col min="16" max="16" width="12.09765625" customWidth="1"/>
-    <col min="21" max="21" width="15.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="4" spans="1:21">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="F4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="J4" s="19" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="J4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="N4" s="19" t="s">
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="N4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="S4" s="19" t="s">
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="S4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1500,7 +1499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
@@ -1614,7 +1613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1633,9 +1632,6 @@
       <c r="P11" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="T12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1655,105 +1651,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1A4EC5-F6CD-4C92-8F27-92D78800539F}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17:P34"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="72" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCellId="1" sqref="I2 A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.09765625" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="4" max="4" width="10.09765625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" customWidth="1"/>
-    <col min="10" max="10" width="19.69921875" customWidth="1"/>
-    <col min="11" max="12" width="11.59765625" customWidth="1"/>
-    <col min="14" max="14" width="13.09765625" customWidth="1"/>
-    <col min="16" max="16" width="12.09765625" customWidth="1"/>
-    <col min="18" max="18" width="16.09765625" customWidth="1"/>
-    <col min="19" max="19" width="11.296875" customWidth="1"/>
-    <col min="20" max="20" width="10.796875" customWidth="1"/>
-    <col min="21" max="21" width="15.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="12" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.77734375" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="4" spans="1:21">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="B6" s="21" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="F6" s="19" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="F6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="J6" s="21" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="J6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="23"/>
-      <c r="N6" s="19" t="s">
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="N6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="R6" s="21" t="s">
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="R6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="23"/>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="S6" s="23"/>
+      <c r="T6" s="24"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1800,7 +1796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1847,7 +1843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1894,7 +1890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1941,7 +1937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1979,7 +1975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2008,7 +2004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
@@ -2028,58 +2024,58 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
-      <c r="B15" s="19" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-    </row>
-    <row r="17" spans="2:20">
-      <c r="B17" s="21" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="F17" s="21" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="F17" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
-      <c r="J17" s="21" t="s">
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="J17" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23"/>
-      <c r="N17" s="21" t="s">
+      <c r="K17" s="23"/>
+      <c r="L17" s="24"/>
+      <c r="N17" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
-      <c r="R17" s="21" t="s">
+      <c r="O17" s="23"/>
+      <c r="P17" s="24"/>
+      <c r="R17" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="S17" s="22"/>
-      <c r="T17" s="23"/>
-    </row>
-    <row r="18" spans="2:20">
+      <c r="S17" s="23"/>
+      <c r="T17" s="24"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -2126,7 +2122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -2173,7 +2169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:20">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2220,7 +2216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:20">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
@@ -2267,7 +2263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:20">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -2305,7 +2301,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:20">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
@@ -2334,7 +2330,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:20">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2344,11 +2340,11 @@
       <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="J24" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="22"/>
-      <c r="L24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
       <c r="N24" s="2" t="s">
         <v>35</v>
       </c>
@@ -2358,13 +2354,13 @@
       <c r="P24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R24" s="21" t="s">
+      <c r="R24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="S24" s="22"/>
-      <c r="T24" s="23"/>
-    </row>
-    <row r="25" spans="2:20">
+      <c r="S24" s="23"/>
+      <c r="T24" s="24"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="J25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2384,7 +2380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:20">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="J26" s="2" t="s">
         <v>16</v>
       </c>
@@ -2394,11 +2390,11 @@
       <c r="L26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="N26" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="24"/>
       <c r="R26" s="2" t="s">
         <v>16</v>
       </c>
@@ -2409,7 +2405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:20">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="J27" s="2" t="s">
         <v>55</v>
       </c>
@@ -2438,7 +2434,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:20">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="J28" s="2" t="s">
         <v>56</v>
       </c>
@@ -2467,7 +2463,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:20">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F29" s="8" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:20">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F30" s="1" t="s">
         <v>13</v>
       </c>
@@ -2493,13 +2489,13 @@
       <c r="H30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="J30" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K30" s="22"/>
-      <c r="L30" s="23"/>
-    </row>
-    <row r="31" spans="2:20">
+      <c r="K30" s="23"/>
+      <c r="L30" s="24"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F31" s="2" t="s">
         <v>16</v>
       </c>
@@ -2518,13 +2514,13 @@
       <c r="L31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N31" s="21" t="s">
+      <c r="N31" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="O31" s="22"/>
-      <c r="P31" s="23"/>
-    </row>
-    <row r="32" spans="2:20">
+      <c r="O31" s="23"/>
+      <c r="P31" s="24"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F32" s="2" t="s">
         <v>19</v>
       </c>
@@ -2553,7 +2549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="10:16">
+    <row r="33" spans="10:16" x14ac:dyDescent="0.3">
       <c r="J33" s="2" t="s">
         <v>57</v>
       </c>
@@ -2573,7 +2569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="10:16">
+    <row r="34" spans="10:16" x14ac:dyDescent="0.3">
       <c r="J34" s="2" t="s">
         <v>19</v>
       </c>
@@ -2593,7 +2589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="10:16">
+    <row r="35" spans="10:16" x14ac:dyDescent="0.3">
       <c r="J35" s="2" t="s">
         <v>58</v>
       </c>
@@ -2606,13 +2602,8 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="R17:T17"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="J30:L30"/>
@@ -2623,8 +2614,13 @@
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2634,108 +2630,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B460EA2-99DC-4461-96FC-6AD0BADF1806}">
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" workbookViewId="0">
+    <sheetView zoomScale="57" workbookViewId="0">
       <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.09765625" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="4" max="4" width="10.09765625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" customWidth="1"/>
-    <col min="10" max="10" width="19.69921875" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" customWidth="1"/>
-    <col min="14" max="14" width="13.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="12.09765625" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
-    <col min="19" max="19" width="11.296875" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
     <col min="20" max="20" width="10" customWidth="1"/>
-    <col min="21" max="21" width="15.09765625" customWidth="1"/>
-    <col min="22" max="23" width="10.69921875" customWidth="1"/>
-    <col min="24" max="24" width="9.8984375" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
+    <col min="22" max="23" width="10.6640625" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="4" spans="1:21">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="B6" s="21" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="F6" s="21" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="F6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="J6" s="21" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="J6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="23"/>
-      <c r="N6" s="21" t="s">
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="N6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="23"/>
-      <c r="R6" s="21" t="s">
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="R6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="23"/>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="S6" s="23"/>
+      <c r="T6" s="24"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -2782,7 +2778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2829,7 +2825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -2876,7 +2872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
@@ -2923,7 +2919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -2961,7 +2957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2990,7 +2986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
@@ -3000,11 +2996,11 @@
       <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="24"/>
       <c r="N13" s="2" t="s">
         <v>35</v>
       </c>
@@ -3014,13 +3010,13 @@
       <c r="P13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R13" s="21" t="s">
+      <c r="R13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="S13" s="22"/>
-      <c r="T13" s="23"/>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="S13" s="23"/>
+      <c r="T13" s="24"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3040,7 +3036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J15" s="2" t="s">
         <v>16</v>
       </c>
@@ -3050,11 +3046,11 @@
       <c r="L15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="N15" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="24"/>
       <c r="R15" s="2" t="s">
         <v>16</v>
       </c>
@@ -3065,7 +3061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J16" s="2" t="s">
         <v>19</v>
       </c>
@@ -3094,7 +3090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:24">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F17" s="8" t="s">
         <v>46</v>
       </c>
@@ -3119,7 +3115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:24">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="s">
         <v>13</v>
       </c>
@@ -3129,11 +3125,11 @@
       <c r="H18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J18" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="24"/>
       <c r="N18" s="2" t="s">
         <v>19</v>
       </c>
@@ -3144,7 +3140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:24">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F19" s="2" t="s">
         <v>16</v>
       </c>
@@ -3164,7 +3160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:24">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F20" s="2" t="s">
         <v>19</v>
       </c>
@@ -3183,13 +3179,13 @@
       <c r="L20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N20" s="21" t="s">
+      <c r="N20" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
-    </row>
-    <row r="21" spans="2:24">
+      <c r="O20" s="23"/>
+      <c r="P20" s="24"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
       <c r="J21" s="2" t="s">
         <v>19</v>
       </c>
@@ -3209,7 +3205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:24">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N22" s="2" t="s">
         <v>16</v>
       </c>
@@ -3220,7 +3216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:24">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3231,63 +3227,63 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:24">
-      <c r="B24" s="19" t="s">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B24" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-    </row>
-    <row r="26" spans="2:24">
-      <c r="B26" s="21" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B26" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="F26" s="21" t="s">
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="F26" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="J26" s="21" t="s">
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
+      <c r="J26" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="22"/>
-      <c r="L26" s="23"/>
-      <c r="N26" s="21" t="s">
+      <c r="K26" s="23"/>
+      <c r="L26" s="24"/>
+      <c r="N26" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
-      <c r="R26" s="21" t="s">
+      <c r="O26" s="23"/>
+      <c r="P26" s="24"/>
+      <c r="R26" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="S26" s="22"/>
-      <c r="T26" s="23"/>
-      <c r="V26" s="21" t="s">
+      <c r="S26" s="23"/>
+      <c r="T26" s="24"/>
+      <c r="V26" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="W26" s="22"/>
-      <c r="X26" s="23"/>
-    </row>
-    <row r="27" spans="2:24">
+      <c r="W26" s="23"/>
+      <c r="X26" s="24"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
@@ -3343,7 +3339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:24">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
@@ -3399,7 +3395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:24">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
@@ -3455,7 +3451,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:24">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>22</v>
       </c>
@@ -3511,7 +3507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:24">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
@@ -3558,7 +3554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:24">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>34</v>
       </c>
@@ -3587,7 +3583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:24">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>36</v>
       </c>
@@ -3597,11 +3593,11 @@
       <c r="D33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="J33" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="K33" s="22"/>
-      <c r="L33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24"/>
       <c r="N33" s="2" t="s">
         <v>35</v>
       </c>
@@ -3611,13 +3607,13 @@
       <c r="P33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V33" s="21" t="s">
+      <c r="V33" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="W33" s="22"/>
-      <c r="X33" s="23"/>
-    </row>
-    <row r="34" spans="2:24">
+      <c r="W33" s="23"/>
+      <c r="X33" s="24"/>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.3">
       <c r="J34" s="1" t="s">
         <v>13</v>
       </c>
@@ -3637,7 +3633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:24">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.3">
       <c r="J35" s="2" t="s">
         <v>16</v>
       </c>
@@ -3647,11 +3643,11 @@
       <c r="L35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N35" s="21" t="s">
+      <c r="N35" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="O35" s="22"/>
-      <c r="P35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="24"/>
       <c r="V35" s="2" t="s">
         <v>16</v>
       </c>
@@ -3662,7 +3658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:24">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.3">
       <c r="J36" s="2" t="s">
         <v>19</v>
       </c>
@@ -3691,12 +3687,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:24">
-      <c r="F37" s="21" t="s">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="F37" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="22"/>
-      <c r="H37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="24"/>
       <c r="N37" s="2" t="s">
         <v>16</v>
       </c>
@@ -3716,7 +3712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:24">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F38" s="1" t="s">
         <v>13</v>
       </c>
@@ -3726,11 +3722,11 @@
       <c r="H38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J38" s="21" t="s">
+      <c r="J38" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K38" s="22"/>
-      <c r="L38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="24"/>
       <c r="N38" s="2" t="s">
         <v>19</v>
       </c>
@@ -3741,7 +3737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="2:24">
+    <row r="39" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F39" s="2" t="s">
         <v>16</v>
       </c>
@@ -3761,7 +3757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:24">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F40" s="2" t="s">
         <v>19</v>
       </c>
@@ -3780,13 +3776,13 @@
       <c r="L40" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N40" s="21" t="s">
+      <c r="N40" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="O40" s="22"/>
-      <c r="P40" s="23"/>
-    </row>
-    <row r="41" spans="2:24">
+      <c r="O40" s="23"/>
+      <c r="P40" s="24"/>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.3">
       <c r="J41" s="2" t="s">
         <v>19</v>
       </c>
@@ -3806,7 +3802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="2:24">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N42" s="2" t="s">
         <v>16</v>
       </c>
@@ -3817,7 +3813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="2:24">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N43" s="2" t="s">
         <v>19</v>
       </c>
@@ -3830,6 +3826,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="V26:X26"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="R26:T26"/>
     <mergeCell ref="N40:P40"/>
     <mergeCell ref="V33:X33"/>
     <mergeCell ref="A1:H1"/>
@@ -3846,16 +3852,6 @@
     <mergeCell ref="R13:T13"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="N20:P20"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="V26:X26"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="N35:P35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>